<commit_message>
Examples (questionnaire, documentation): Added measurement information.
</commit_message>
<xml_diff>
--- a/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
+++ b/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="14380" yWindow="6320" windowWidth="26580" windowHeight="20020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="14380" yWindow="6320" windowWidth="26580" windowHeight="20020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="larceny" sheetId="1" r:id="rId1"/>
     <sheet name="guile" sheetId="2" r:id="rId2"/>
+    <sheet name="configuration" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
   <si>
     <t>3_1</t>
   </si>
@@ -83,6 +84,39 @@
   </si>
   <si>
     <t>computed</t>
+  </si>
+  <si>
+    <t>Version:</t>
+  </si>
+  <si>
+    <t>GNU Guile 2.0.11</t>
+  </si>
+  <si>
+    <t>0.98 "General Ripper"</t>
+  </si>
+  <si>
+    <t>MacBook Air (Mid 2011)</t>
+  </si>
+  <si>
+    <t>1.7 GHz Intel Core i5</t>
+  </si>
+  <si>
+    <t>4 GB @ 1333 MHz DDR3</t>
+  </si>
+  <si>
+    <t>CPU:</t>
+  </si>
+  <si>
+    <t>RAM:</t>
+  </si>
+  <si>
+    <t>OS:</t>
+  </si>
+  <si>
+    <t>Notebook:</t>
+  </si>
+  <si>
+    <t>Mac OS 10.10.4</t>
   </si>
 </sst>
 </file>
@@ -187,7 +221,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="169">
+  <cellStyleXfs count="171">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -357,8 +391,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -404,8 +440,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="169">
+  <cellStyles count="171">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -490,6 +529,7 @@
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -574,6 +614,7 @@
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -905,9 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1596,6 +1635,14 @@
         <v>0.26813186813186812</v>
       </c>
       <c r="J26" s="16"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="B32" s="2"/>
@@ -1632,7 +1679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2321,6 +2368,14 @@
         <v>0.48091801235785864</v>
       </c>
       <c r="J26" s="16"/>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" spans="1:10">
       <c r="B32" s="2"/>
@@ -2351,4 +2406,57 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Examples (ttc-2015-fuml-activity-diagrams): Final profiling; added measurements if enabled analysis is not cached.
</commit_message>
<xml_diff>
--- a/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
+++ b/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="36">
   <si>
     <t>3_1</t>
   </si>
@@ -118,19 +118,16 @@
     <t>Incremental savings (use enabled passes)</t>
   </si>
   <si>
-    <t>Iterations (use enabled passes)</t>
-  </si>
-  <si>
     <t>task</t>
   </si>
   <si>
-    <t>Transitions on average checked (no enabled passes)</t>
-  </si>
-  <si>
-    <t>Number of transitions</t>
-  </si>
-  <si>
     <t>Larceny 0.98 "General Ripper"</t>
+  </si>
+  <si>
+    <t>Petri net execution (no caching, no enabled passes)</t>
+  </si>
+  <si>
+    <t>Petri net execution (no caching, use enabled passes)</t>
   </si>
 </sst>
 </file>
@@ -250,8 +247,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="261">
+  <cellStyleXfs count="295">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -548,22 +579,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -575,17 +594,24 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -593,8 +619,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="261">
+  <cellStyles count="295">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -725,6 +756,23 @@
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="294" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -855,6 +903,23 @@
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="293" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1184,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1197,32 +1262,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
     </row>
     <row r="2" spans="1:10">
-      <c r="B2" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="16">
+      <c r="B2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="15">
         <v>1</v>
       </c>
-      <c r="D2" s="16">
+      <c r="D2" s="15">
         <v>2</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="28" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1240,12 +1305,12 @@
       <c r="F3" s="6">
         <v>641</v>
       </c>
-      <c r="J3" s="29" t="s">
+      <c r="J3" s="25" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="31"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1261,10 +1326,10 @@
       <c r="F4" s="6">
         <v>643</v>
       </c>
-      <c r="J4" s="29"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="31"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1281,10 +1346,10 @@
         <v>647</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="J5" s="29"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="31"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1301,10 +1366,10 @@
         <v>655</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="J6" s="29"/>
+      <c r="J6" s="25"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="31"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1321,7 +1386,7 @@
         <v>656</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="J7" s="29"/>
+      <c r="J7" s="25"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="12" t="s">
@@ -1342,7 +1407,7 @@
       <c r="F8" s="6">
         <v>699</v>
       </c>
-      <c r="J8" s="29"/>
+      <c r="J8" s="25"/>
     </row>
     <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="13" t="s">
@@ -1366,10 +1431,10 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="29"/>
+      <c r="J9" s="25"/>
     </row>
     <row r="10" spans="1:10" ht="16" thickTop="1">
-      <c r="A10" s="32" t="s">
+      <c r="A10" s="29" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1391,12 +1456,12 @@
         <f>F3</f>
         <v>641</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="31"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1416,10 +1481,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J11" s="27"/>
+      <c r="J11" s="26"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="31"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1439,10 +1504,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="26"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="31"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1462,10 +1527,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J13" s="27"/>
+      <c r="J13" s="26"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="31"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1485,7 +1550,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J14" s="27"/>
+      <c r="J14" s="26"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="7" t="s">
@@ -1510,7 +1575,7 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="J15" s="27"/>
+      <c r="J15" s="26"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="7" t="s">
@@ -1535,10 +1600,10 @@
         <f>F9-F7</f>
         <v>62</v>
       </c>
-      <c r="J16" s="27"/>
+      <c r="J16" s="26"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="28" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1553,10 +1618,10 @@
       <c r="I17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="27"/>
+      <c r="J17" s="26"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="31"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1588,10 +1653,10 @@
         <f>SUM(C10:F10)/SUM(C8:F8)</f>
         <v>0.5254477744280901</v>
       </c>
-      <c r="J18" s="27"/>
+      <c r="J18" s="26"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="31"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1623,10 +1688,10 @@
         <f>SUM(C11:F11)/SUM(C8:F8)</f>
         <v>6.9338535201276821E-2</v>
       </c>
-      <c r="J19" s="27"/>
+      <c r="J19" s="26"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="31"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1658,10 +1723,10 @@
         <f>SUM(C12:F12)/SUM(C8:F8)</f>
         <v>6.7387834722468523E-2</v>
       </c>
-      <c r="J20" s="27"/>
+      <c r="J20" s="26"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="31"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
@@ -1693,10 +1758,10 @@
         <f>SUM(C13:F13)/SUM(C8:F8)</f>
         <v>9.1505586096825672E-2</v>
       </c>
-      <c r="J21" s="27"/>
+      <c r="J21" s="26"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="31"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
@@ -1728,10 +1793,10 @@
         <f>SUM(C14:F14)/SUM(C8:F8)</f>
         <v>2.3763078560028374E-2</v>
       </c>
-      <c r="J22" s="27"/>
+      <c r="J22" s="26"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="31"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
@@ -1763,10 +1828,10 @@
         <f>SUM(C15:F15)/SUM(C8:F8)</f>
         <v>0.22255719099131052</v>
       </c>
-      <c r="J23" s="27"/>
+      <c r="J23" s="26"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="28" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1781,10 +1846,10 @@
       <c r="I24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="27"/>
+      <c r="J24" s="26"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="31"/>
+      <c r="A25" s="28"/>
       <c r="B25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1816,10 +1881,10 @@
         <f>SUM(C10:F10)/SUM(C9:F9)</f>
         <v>0.52137955305296502</v>
       </c>
-      <c r="J25" s="27"/>
+      <c r="J25" s="26"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="31"/>
+      <c r="A26" s="28"/>
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1851,10 +1916,10 @@
         <f>SUM(C11:F11)/SUM(C9:F9)</f>
         <v>6.8801689248636277E-2</v>
       </c>
-      <c r="J26" s="27"/>
+      <c r="J26" s="26"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="31"/>
+      <c r="A27" s="28"/>
       <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
@@ -1886,10 +1951,10 @@
         <f>SUM(C12:F12)/SUM(C9:F9)</f>
         <v>6.6866091852894605E-2</v>
       </c>
-      <c r="J27" s="27"/>
+      <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="31"/>
+      <c r="A28" s="28"/>
       <c r="B28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1921,10 +1986,10 @@
         <f>SUM(C13:F13)/SUM(C9:F9)</f>
         <v>9.0797114200246345E-2</v>
       </c>
-      <c r="J28" s="27"/>
+      <c r="J28" s="26"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="31"/>
+      <c r="A29" s="28"/>
       <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
@@ -1956,10 +2021,10 @@
         <f>SUM(C14:F14)/SUM(C9:F9)</f>
         <v>2.357909554812599E-2</v>
       </c>
-      <c r="J29" s="27"/>
+      <c r="J29" s="26"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="31"/>
+      <c r="A30" s="28"/>
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
@@ -1991,193 +2056,318 @@
         <f>SUM(C16:F16)/SUM(C9:F9)</f>
         <v>0.22857645609713179</v>
       </c>
-      <c r="J30" s="27"/>
-    </row>
-    <row r="31" spans="1:10" ht="6" customHeight="1">
-      <c r="A31" s="23"/>
-      <c r="B31" s="24"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="26"/>
-    </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="15"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="28" t="s">
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="22"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="16"/>
+    </row>
+    <row r="32" spans="1:10" ht="5" customHeight="1">
+      <c r="A32" s="17"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="20"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="22"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="16"/>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="22"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="20"/>
-    </row>
-    <row r="33" spans="1:10">
-      <c r="C33" s="16">
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="27"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="16"/>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="22"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="21">
         <v>1</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D35" s="21">
         <v>2</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E35" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="F33" s="16" t="s">
+      <c r="F35" s="21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10">
-      <c r="B34" s="21" t="s">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="16"/>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="6">
+        <v>9894</v>
+      </c>
+      <c r="D36" s="6">
+        <v>8171</v>
+      </c>
+      <c r="E36" s="6">
+        <v>8707</v>
+      </c>
+      <c r="F36" s="6">
+        <v>916</v>
+      </c>
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="16" thickBot="1">
+      <c r="A37" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="22">
-        <v>1002</v>
-      </c>
-      <c r="D34" s="22">
-        <v>1004</v>
-      </c>
-      <c r="E34" s="22">
-        <v>1004</v>
-      </c>
-      <c r="F34" s="22">
-        <v>1000</v>
-      </c>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10">
-      <c r="B35" s="17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C35" s="18">
-        <v>1002</v>
-      </c>
-      <c r="D35" s="18">
-        <v>14</v>
-      </c>
-      <c r="E35" s="18">
-        <v>14</v>
-      </c>
-      <c r="F35" s="18">
-        <v>1000</v>
-      </c>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="30"/>
-    </row>
-    <row r="36" spans="1:10" ht="16" thickBot="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="9" t="s">
+      <c r="C37" s="10">
+        <v>18889</v>
+      </c>
+      <c r="D37" s="10">
+        <v>1536</v>
+      </c>
+      <c r="E37" s="10">
+        <v>1818</v>
+      </c>
+      <c r="F37" s="10">
+        <v>1057</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="24"/>
+      <c r="I37" s="24"/>
+      <c r="J37" s="25"/>
+    </row>
+    <row r="38" spans="1:12" ht="16" thickTop="1">
+      <c r="A38" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="10">
-        <f>C34/2+0.5</f>
-        <v>501.5</v>
-      </c>
-      <c r="D36" s="10">
-        <v>172.5</v>
-      </c>
-      <c r="E36" s="10">
-        <v>172.5</v>
-      </c>
-      <c r="F36" s="10">
-        <f>F34/2+0.5</f>
-        <v>500.5</v>
-      </c>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="30"/>
-    </row>
-    <row r="37" spans="1:10" ht="16" thickTop="1">
-      <c r="B37" s="5" t="s">
+      <c r="C38" s="31">
+        <f>C36-C7</f>
+        <v>8727</v>
+      </c>
+      <c r="D38" s="31">
+        <f>D36-D7</f>
+        <v>6986</v>
+      </c>
+      <c r="E38" s="31">
+        <f>E36-E7</f>
+        <v>7331</v>
+      </c>
+      <c r="F38" s="31">
+        <f>F36-F7</f>
+        <v>260</v>
+      </c>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
+      <c r="I38" s="31"/>
+      <c r="J38" s="26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" s="31">
+        <f>C37-C7</f>
+        <v>17722</v>
+      </c>
+      <c r="D39" s="31">
+        <f>D37-D7</f>
+        <v>351</v>
+      </c>
+      <c r="E39" s="31">
+        <f>E37-E7</f>
+        <v>442</v>
+      </c>
+      <c r="F39" s="31">
+        <f>F37-F7</f>
+        <v>401</v>
+      </c>
+      <c r="G39" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="H39" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="26"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="22"/>
+      <c r="B40" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C37" s="3">
-        <f>1-C15/(C34*C36*(C14/C34))</f>
-        <v>0.96548815093181994</v>
-      </c>
-      <c r="D37" s="3">
-        <f>1-D15/(D34*D36*(D14/D34))</f>
-        <v>0.92055823939881909</v>
-      </c>
-      <c r="E37" s="3">
-        <f>1-E15/(E34*E36*(E14/E34))</f>
-        <v>0.9715942028985507</v>
-      </c>
-      <c r="F37" s="3">
-        <f>1-F15/(F34*F36*(F14/F34))</f>
-        <v>0.91408591408591411</v>
-      </c>
-      <c r="J37" s="27" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10">
-      <c r="B38" s="5" t="s">
+      <c r="C40" s="3">
+        <f>(C38-C15)/C38</f>
+        <v>0.9484358886215194</v>
+      </c>
+      <c r="D40" s="3">
+        <f>(D38-D15)/D38</f>
+        <v>0.94703693100486686</v>
+      </c>
+      <c r="E40" s="3">
+        <f>(E38-E15)/E38</f>
+        <v>0.94652844086754873</v>
+      </c>
+      <c r="F40" s="3">
+        <f>(F38-F15)/F38</f>
+        <v>0.83461538461538465</v>
+      </c>
+      <c r="G40" s="3">
+        <f>MIN(C40:F40)</f>
+        <v>0.83461538461538465</v>
+      </c>
+      <c r="H40" s="3">
+        <f>MAX(C40:F40)</f>
+        <v>0.9484358886215194</v>
+      </c>
+      <c r="I40" s="3">
+        <f>(SUM(C38:F38)-SUM(C15:F15))/SUM(C38:F38)</f>
+        <v>0.9461465842773773</v>
+      </c>
+      <c r="J40" s="26"/>
+      <c r="L40" s="3"/>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="22"/>
+      <c r="B41" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C38" s="3">
-        <f>1-C16/(C14*C35)</f>
-        <v>0.95750806080147399</v>
-      </c>
-      <c r="D38" s="3">
-        <f>1-D16/(D14*D35)</f>
-        <v>0.8835978835978836</v>
-      </c>
-      <c r="E38" s="3">
-        <f>1-E16/(E14*E35)</f>
-        <v>0.92321428571428577</v>
-      </c>
-      <c r="F38" s="3">
-        <f>1-F16/(F14*F35)</f>
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="J38" s="27"/>
-    </row>
-    <row r="40" spans="1:10">
-      <c r="A40" s="4" t="s">
+      <c r="C41" s="3">
+        <f>(C39-C16)/C39</f>
+        <v>0.93753526689989841</v>
+      </c>
+      <c r="D41" s="3">
+        <f>(D39-D16)/D39</f>
+        <v>0.87464387464387461</v>
+      </c>
+      <c r="E41" s="3">
+        <f>(E39-E16)/E39</f>
+        <v>0.80542986425339369</v>
+      </c>
+      <c r="F41" s="3">
+        <f>(F39-F16)/F39</f>
+        <v>0.84538653366583538</v>
+      </c>
+      <c r="G41" s="3">
+        <f>MIN(C41:F41)</f>
+        <v>0.80542986425339369</v>
+      </c>
+      <c r="H41" s="3">
+        <f>MAX(C41:F41)</f>
+        <v>0.93753526689989841</v>
+      </c>
+      <c r="I41" s="3">
+        <f>(SUM(C39:F39)-SUM(C16:F16))/SUM(C39:F39)</f>
+        <v>0.9313279763163459</v>
+      </c>
+      <c r="J41" s="26"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="22"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="16"/>
+    </row>
+    <row r="43" spans="1:12" ht="5" customHeight="1">
+      <c r="A43" s="17"/>
+      <c r="B43" s="18"/>
+      <c r="C43" s="19"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="19"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="19"/>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10">
-      <c r="B44" s="2"/>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="8" t="s">
+      <c r="B45" s="14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2">
+      <c r="B49" s="2"/>
+    </row>
+    <row r="67" spans="2:2">
+      <c r="B67" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="8"/>
+    <row r="68" spans="2:2">
+      <c r="B68" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J38:J41"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="A17:A23"/>
     <mergeCell ref="A24:A30"/>
     <mergeCell ref="A3:A7"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="C32:F32"/>
     <mergeCell ref="J3:J9"/>
     <mergeCell ref="J10:J30"/>
-    <mergeCell ref="J34:J36"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="J36:J37"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Examples (ttc-2015-fuml-activity-diagrams documentation): Fixed minor spelling and consistency errors.
</commit_message>
<xml_diff>
--- a/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
+++ b/examples/ttc-2015-fuml-activity-diagrams/documentation/figures/measurements.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27022"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="820" yWindow="300" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
@@ -109,9 +109,6 @@
     <t>Petri net enabled</t>
   </si>
   <si>
-    <t>Mac OS 10.11.3</t>
-  </si>
-  <si>
     <t>Incremental savings (no enabled passes)</t>
   </si>
   <si>
@@ -128,6 +125,9 @@
   </si>
   <si>
     <t>Petri net execution (no caching, use enabled passes)</t>
+  </si>
+  <si>
+    <t>Mac OS 10.11.5</t>
   </si>
 </sst>
 </file>
@@ -604,9 +604,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -619,11 +621,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="295">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I41" sqref="I41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1262,16 +1262,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
     </row>
     <row r="2" spans="1:10">
       <c r="B2" s="15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="15">
         <v>1</v>
@@ -1287,7 +1287,7 @@
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1305,12 +1305,12 @@
       <c r="F3" s="6">
         <v>641</v>
       </c>
-      <c r="J3" s="25" t="s">
+      <c r="J3" s="32" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="28"/>
+      <c r="A4" s="30"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1326,10 +1326,10 @@
       <c r="F4" s="6">
         <v>643</v>
       </c>
-      <c r="J4" s="25"/>
+      <c r="J4" s="32"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="28"/>
+      <c r="A5" s="30"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
@@ -1346,10 +1346,10 @@
         <v>647</v>
       </c>
       <c r="G5" s="6"/>
-      <c r="J5" s="25"/>
+      <c r="J5" s="32"/>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="28"/>
+      <c r="A6" s="30"/>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1366,10 +1366,10 @@
         <v>655</v>
       </c>
       <c r="G6" s="6"/>
-      <c r="J6" s="25"/>
+      <c r="J6" s="32"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="28"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="5" t="s">
         <v>28</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>656</v>
       </c>
       <c r="G7" s="6"/>
-      <c r="J7" s="25"/>
+      <c r="J7" s="32"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="12" t="s">
@@ -1407,7 +1407,7 @@
       <c r="F8" s="6">
         <v>699</v>
       </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="32"/>
     </row>
     <row r="9" spans="1:10" ht="16" thickBot="1">
       <c r="A9" s="13" t="s">
@@ -1431,10 +1431,10 @@
       <c r="G9" s="11"/>
       <c r="H9" s="11"/>
       <c r="I9" s="11"/>
-      <c r="J9" s="25"/>
+      <c r="J9" s="32"/>
     </row>
     <row r="10" spans="1:10" ht="16" thickTop="1">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="31" t="s">
         <v>26</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -1456,12 +1456,12 @@
         <f>F3</f>
         <v>641</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="28" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="28"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="5" t="s">
         <v>3</v>
       </c>
@@ -1481,10 +1481,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="J11" s="26"/>
+      <c r="J11" s="28"/>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="28"/>
+      <c r="A12" s="30"/>
       <c r="B12" s="5" t="s">
         <v>4</v>
       </c>
@@ -1504,10 +1504,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="28"/>
+      <c r="A13" s="30"/>
       <c r="B13" s="5" t="s">
         <v>5</v>
       </c>
@@ -1527,10 +1527,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="J13" s="26"/>
+      <c r="J13" s="28"/>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="28"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="5" t="s">
         <v>28</v>
       </c>
@@ -1550,7 +1550,7 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J14" s="26"/>
+      <c r="J14" s="28"/>
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="7" t="s">
@@ -1575,7 +1575,7 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="J15" s="26"/>
+      <c r="J15" s="28"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="7" t="s">
@@ -1600,10 +1600,10 @@
         <f>F9-F7</f>
         <v>62</v>
       </c>
-      <c r="J16" s="26"/>
+      <c r="J16" s="28"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="30" t="s">
         <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1618,10 +1618,10 @@
       <c r="I17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="26"/>
+      <c r="J17" s="28"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="28"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="5" t="s">
         <v>2</v>
       </c>
@@ -1653,10 +1653,10 @@
         <f>SUM(C10:F10)/SUM(C8:F8)</f>
         <v>0.5254477744280901</v>
       </c>
-      <c r="J18" s="26"/>
+      <c r="J18" s="28"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="28"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="5" t="s">
         <v>3</v>
       </c>
@@ -1688,10 +1688,10 @@
         <f>SUM(C11:F11)/SUM(C8:F8)</f>
         <v>6.9338535201276821E-2</v>
       </c>
-      <c r="J19" s="26"/>
+      <c r="J19" s="28"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="28"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1723,10 +1723,10 @@
         <f>SUM(C12:F12)/SUM(C8:F8)</f>
         <v>6.7387834722468523E-2</v>
       </c>
-      <c r="J20" s="26"/>
+      <c r="J20" s="28"/>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="28"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="5" t="s">
         <v>5</v>
       </c>
@@ -1758,10 +1758,10 @@
         <f>SUM(C13:F13)/SUM(C8:F8)</f>
         <v>9.1505586096825672E-2</v>
       </c>
-      <c r="J21" s="26"/>
+      <c r="J21" s="28"/>
     </row>
     <row r="22" spans="1:10">
-      <c r="A22" s="28"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="5" t="s">
         <v>28</v>
       </c>
@@ -1793,10 +1793,10 @@
         <f>SUM(C14:F14)/SUM(C8:F8)</f>
         <v>2.3763078560028374E-2</v>
       </c>
-      <c r="J22" s="26"/>
+      <c r="J22" s="28"/>
     </row>
     <row r="23" spans="1:10">
-      <c r="A23" s="28"/>
+      <c r="A23" s="30"/>
       <c r="B23" s="5" t="s">
         <v>11</v>
       </c>
@@ -1828,10 +1828,10 @@
         <f>SUM(C15:F15)/SUM(C8:F8)</f>
         <v>0.22255719099131052</v>
       </c>
-      <c r="J23" s="26"/>
+      <c r="J23" s="28"/>
     </row>
     <row r="24" spans="1:10">
-      <c r="A24" s="28" t="s">
+      <c r="A24" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -1846,10 +1846,10 @@
       <c r="I24" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="26"/>
+      <c r="J24" s="28"/>
     </row>
     <row r="25" spans="1:10">
-      <c r="A25" s="28"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="5" t="s">
         <v>2</v>
       </c>
@@ -1881,10 +1881,10 @@
         <f>SUM(C10:F10)/SUM(C9:F9)</f>
         <v>0.52137955305296502</v>
       </c>
-      <c r="J25" s="26"/>
+      <c r="J25" s="28"/>
     </row>
     <row r="26" spans="1:10">
-      <c r="A26" s="28"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="5" t="s">
         <v>3</v>
       </c>
@@ -1916,10 +1916,10 @@
         <f>SUM(C11:F11)/SUM(C9:F9)</f>
         <v>6.8801689248636277E-2</v>
       </c>
-      <c r="J26" s="26"/>
+      <c r="J26" s="28"/>
     </row>
     <row r="27" spans="1:10">
-      <c r="A27" s="28"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="5" t="s">
         <v>4</v>
       </c>
@@ -1951,10 +1951,10 @@
         <f>SUM(C12:F12)/SUM(C9:F9)</f>
         <v>6.6866091852894605E-2</v>
       </c>
-      <c r="J27" s="26"/>
+      <c r="J27" s="28"/>
     </row>
     <row r="28" spans="1:10">
-      <c r="A28" s="28"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="5" t="s">
         <v>5</v>
       </c>
@@ -1986,10 +1986,10 @@
         <f>SUM(C13:F13)/SUM(C9:F9)</f>
         <v>9.0797114200246345E-2</v>
       </c>
-      <c r="J28" s="26"/>
+      <c r="J28" s="28"/>
     </row>
     <row r="29" spans="1:10">
-      <c r="A29" s="28"/>
+      <c r="A29" s="30"/>
       <c r="B29" s="5" t="s">
         <v>28</v>
       </c>
@@ -2021,10 +2021,10 @@
         <f>SUM(C14:F14)/SUM(C9:F9)</f>
         <v>2.357909554812599E-2</v>
       </c>
-      <c r="J29" s="26"/>
+      <c r="J29" s="28"/>
     </row>
     <row r="30" spans="1:10">
-      <c r="A30" s="28"/>
+      <c r="A30" s="30"/>
       <c r="B30" s="5" t="s">
         <v>12</v>
       </c>
@@ -2056,7 +2056,7 @@
         <f>SUM(C16:F16)/SUM(C9:F9)</f>
         <v>0.22857645609713179</v>
       </c>
-      <c r="J30" s="26"/>
+      <c r="J30" s="28"/>
     </row>
     <row r="31" spans="1:10">
       <c r="A31" s="22"/>
@@ -2097,12 +2097,12 @@
     <row r="34" spans="1:12">
       <c r="A34" s="22"/>
       <c r="B34" s="5"/>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27"/>
-      <c r="F34" s="27"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -2133,7 +2133,7 @@
         <v>15</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="6">
         <v>9894</v>
@@ -2150,7 +2150,7 @@
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
-      <c r="J36" s="25" t="s">
+      <c r="J36" s="32" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2159,7 +2159,7 @@
         <v>27</v>
       </c>
       <c r="B37" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="10">
         <v>18889</v>
@@ -2176,35 +2176,35 @@
       <c r="G37" s="24"/>
       <c r="H37" s="24"/>
       <c r="I37" s="24"/>
-      <c r="J37" s="25"/>
+      <c r="J37" s="32"/>
     </row>
     <row r="38" spans="1:12" ht="16" thickTop="1">
       <c r="A38" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="31">
+        <v>33</v>
+      </c>
+      <c r="C38" s="26">
         <f>C36-C7</f>
         <v>8727</v>
       </c>
-      <c r="D38" s="31">
+      <c r="D38" s="26">
         <f>D36-D7</f>
         <v>6986</v>
       </c>
-      <c r="E38" s="31">
+      <c r="E38" s="26">
         <f>E36-E7</f>
         <v>7331</v>
       </c>
-      <c r="F38" s="31">
+      <c r="F38" s="26">
         <f>F36-F7</f>
         <v>260</v>
       </c>
-      <c r="G38" s="31"/>
-      <c r="H38" s="31"/>
-      <c r="I38" s="31"/>
-      <c r="J38" s="26" t="s">
+      <c r="G38" s="26"/>
+      <c r="H38" s="26"/>
+      <c r="I38" s="26"/>
+      <c r="J38" s="28" t="s">
         <v>17</v>
       </c>
     </row>
@@ -2212,55 +2212,55 @@
       <c r="A39" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="C39" s="31">
+      <c r="B39" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="26">
         <f>C37-C7</f>
         <v>17722</v>
       </c>
-      <c r="D39" s="31">
+      <c r="D39" s="26">
         <f>D37-D7</f>
         <v>351</v>
       </c>
-      <c r="E39" s="31">
+      <c r="E39" s="26">
         <f>E37-E7</f>
         <v>442</v>
       </c>
-      <c r="F39" s="31">
+      <c r="F39" s="26">
         <f>F37-F7</f>
         <v>401</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="H39" s="32" t="s">
+      <c r="H39" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I39" s="32" t="s">
+      <c r="I39" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="J39" s="26"/>
+      <c r="J39" s="28"/>
     </row>
     <row r="40" spans="1:12">
       <c r="A40" s="22"/>
       <c r="B40" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C40" s="3">
-        <f>(C38-C15)/C38</f>
+        <f t="shared" ref="C40:F41" si="5">(C38-C15)/C38</f>
         <v>0.9484358886215194</v>
       </c>
       <c r="D40" s="3">
-        <f>(D38-D15)/D38</f>
+        <f t="shared" si="5"/>
         <v>0.94703693100486686</v>
       </c>
       <c r="E40" s="3">
-        <f>(E38-E15)/E38</f>
+        <f t="shared" si="5"/>
         <v>0.94652844086754873</v>
       </c>
       <c r="F40" s="3">
-        <f>(F38-F15)/F38</f>
+        <f t="shared" si="5"/>
         <v>0.83461538461538465</v>
       </c>
       <c r="G40" s="3">
@@ -2275,28 +2275,28 @@
         <f>(SUM(C38:F38)-SUM(C15:F15))/SUM(C38:F38)</f>
         <v>0.9461465842773773</v>
       </c>
-      <c r="J40" s="26"/>
+      <c r="J40" s="28"/>
       <c r="L40" s="3"/>
     </row>
     <row r="41" spans="1:12">
       <c r="A41" s="22"/>
       <c r="B41" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="3">
-        <f>(C39-C16)/C39</f>
+        <f t="shared" si="5"/>
         <v>0.93753526689989841</v>
       </c>
       <c r="D41" s="3">
-        <f>(D39-D16)/D39</f>
+        <f t="shared" si="5"/>
         <v>0.87464387464387461</v>
       </c>
       <c r="E41" s="3">
-        <f>(E39-E16)/E39</f>
+        <f t="shared" si="5"/>
         <v>0.80542986425339369</v>
       </c>
       <c r="F41" s="3">
-        <f>(F39-F16)/F39</f>
+        <f t="shared" si="5"/>
         <v>0.84538653366583538</v>
       </c>
       <c r="G41" s="3">
@@ -2311,7 +2311,7 @@
         <f>(SUM(C39:F39)-SUM(C16:F16))/SUM(C39:F39)</f>
         <v>0.9313279763163459</v>
       </c>
-      <c r="J41" s="26"/>
+      <c r="J41" s="28"/>
     </row>
     <row r="42" spans="1:12">
       <c r="A42" s="22"/>
@@ -2342,7 +2342,7 @@
         <v>18</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="2:2">
@@ -2383,7 +2383,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -2419,7 +2421,7 @@
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>